<commit_message>
updating excel checklist file
had a format error before, fixed
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Coding\Project\python\Self-Project\ordered\Checklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F467369F-5195-45B2-B430-2774A11B5394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1442591D-B047-47F7-82CC-9C74E74D8A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B679EF15-A35F-43FE-B7D2-F2BE67EA73A7}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="3" activeTab="3" xr2:uid="{B679EF15-A35F-43FE-B7D2-F2BE67EA73A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Trước khi nổ máy" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="146">
   <si>
     <r>
       <t>ENGINE START PREPARATION</t>
@@ -151,20 +151,6 @@
   </si>
   <si>
     <r>
-      <t>Cockpit Lighting ....................................................... As required</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Dome light should be selected on as it is available in EMER ELEC configuration.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Scan Sequence ............................................................. PERFORM</t>
     </r>
     <r>
@@ -233,260 +219,28 @@
     </r>
   </si>
   <si>
-    <t>APU BLEED Pushbutton ..........................................................ON</t>
-  </si>
-  <si>
-    <t>EFIS........................................................... ON/Adjust brightness</t>
-  </si>
-  <si>
-    <r>
-      <t>ADIRS Mode Rotary Selectors............................................NAV</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>IRS IN ALIGN&gt; 7MN appears on ECAM MEMO page.</t>
-    </r>
-  </si>
-  <si>
     <t>Cockpit man</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Fuel On Board (ECAM E/WD) ..........................................NOTE
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Calculate Fuel Qty to make sure after engine shutdown there should be at least 3000 kgs of fuel on board for</t>
-    </r>
-  </si>
-  <si>
     <t>APU BLEED Pushbutton............................................................. ON</t>
   </si>
   <si>
     <t>EFIS ..............................................................ON/Adjust brightness</t>
   </si>
   <si>
-    <r>
-      <t>ADIRS Mode Rotary Selectors ...............................................NAV</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>IRS IN ALIGN&gt; 7MN appears on ECAM MEMO page.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Fuel On Board (ECAM E/WD)............................................. NOTE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Calculate Fuel Qty to make sure after engine shutdown there should be at least 3000 kgs of fuel on board for stability reasons.</t>
-    </r>
-  </si>
-  <si>
     <t>A/SKID &amp; N/W STRG Switch .................................................... ON</t>
   </si>
   <si>
-    <r>
-      <t>RMP 2 ................................................................................. Check ON</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>. SEL and NAV lights extinguished.. Set frequencies as required.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ACP 2 .............................................................................................. INT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>· Check transmission and reception with ground crew.</t>
-    </r>
-  </si>
-  <si>
     <t>Recorder Ground Control ........................................As required</t>
   </si>
   <si>
     <t>SPEED BRAKE Lever .....................................Retract/Disarmed</t>
   </si>
   <si>
-    <r>
-      <t>FLAPS Lever Position ......................................................... CHECK</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>If lever does not agree with flaps/slats indication on ECAM E/WD, set flaps lever to corresponding position.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ECAM Control Panel .....................................................Select HYD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Check hydraulic quantities in normal range, no AIR LOW PRESS warnings.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ECAM Control Panel ................................................... Select FUEL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Check fuel distribution.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ECAM Control Panel ...................................................... Select STS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Check if inoperable systems are compatible for engine run-up.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ECAM Control Panel ......................................................Select CLR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Select CLR as many times as necessary until ECAM DOOR/OXY page appears.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>PARKING BRK ............................................................................. ON</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Check parking brake pressure indication normal.</t>
-    </r>
-  </si>
-  <si>
     <t>NW STRG DISC MEMO..........................................................CHECK</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">MCDU 1 (2).................................................................................... ON
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Check data base validity.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>MCDU................................................................................ Select INIT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Insert airport ICAO reference using keyboard. (VVTS/VVTS for</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>MCDU 1 (2)..................................................................................... ON</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Check data base validity.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>MCDU ............................................................................... Select INIT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Insert airport ICAO reference using keyboard. (VVTS/VVTS for SGN station)MCDU/INIT, select Next Page.Select ALIGN IRS prompt to complete IRS alignment.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>BEFORE ENGINE START</t>
     </r>
     <r>
@@ -522,65 +276,6 @@
       </rPr>
       <t>. SQUIB and DISCH lights extinguished.</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>ENG 1 (2) FIRE TEST ............................. PERFORM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>- Check:. ENG 1 (2) FIRE pushbutton light illuminates.· SQUIB and DISCH lights illuminate.· MASTER WARNING illuminated.· ENG 1 (2) FIRE warning on ECAM E/WD.. CRC sounds.. ECAM ENG page appears.. FIRE 1 (2) light illuminates.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>FADEC Ground Power (both)........................... ON</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>· On E/WD, check all indications normal.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ECAM Control Panel ..............................Select ENG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>· Check all engine parameters for logical indication and sufficient oil quantity.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ECAM Control Panel ..............................Select ENG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>· ECAM DOOR/OXY page appears, check all doors closed.</t>
-    </r>
-  </si>
-  <si>
-    <t>FADEC Ground Power (both) .........................OFFATC Clearance ............................................. OBTAIN</t>
   </si>
   <si>
     <t>Thrust Levers .................... Idle/Reverse Stowed</t>
@@ -868,9 +563,6 @@
     <t>APU or Ext/ Pwr………………………………………………..ON</t>
   </si>
   <si>
-    <t>APU BLEED or HOT AIR BLEED (If APU is INOP)………..ONCheck Bleed Air Pressure is sufficient for Dry Crank.</t>
-  </si>
-  <si>
     <t>MASTER SW………………………………………………….OFF</t>
   </si>
   <si>
@@ -883,25 +575,562 @@
     <t>CO-ERU CALL MECH, SGNBASE…CONFIRM WHICH ENG FIRE</t>
   </si>
   <si>
-    <r>
-      <t>Thrust Levers (both).......................................................... IDLE</t>
-    </r>
-    <r>
-      <rPr>
+    <t>PARKING BRK ...................................................................... ON</t>
+  </si>
+  <si>
+    <t>AGENT 1 &amp; 2 Pushbutton (affected engine)..................PRESS</t>
+  </si>
+  <si>
+    <t>ENG MASTER Switch (other engine) ............................... OFF</t>
+  </si>
+  <si>
+    <t>Quan sát động cơ, nếu hiện tượng cháy vẫn tiếp tục và lan ra phía ngoài cowl động cơ, Headset man cho triển khai phun dập cháy từ bên ngoài động cơ.</t>
+  </si>
+  <si>
+    <t>Yêu cầu nhân viên trực cứu hỏa (Fire Guard) tiến hành dập cháy động cơ.</t>
+  </si>
+  <si>
+    <t>Fire Guard</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NV trực cứu hỏa tiếp cận xịt bình cứu hỏa CO2 vào khu vực cháy trên động cơ. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
+      <t>Lưu ý không xịt vào Engine Inlet/Exhaust.</t>
+    </r>
+  </si>
+  <si>
+    <t>APU FIRE Pushbutton ............................................. RELEASE</t>
+  </si>
+  <si>
+    <t>ADIRS Mode Rotary Selectors ........................................... OFF</t>
+  </si>
+  <si>
+    <t>EXT PWR Pushbutton ........................................................ OFF</t>
+  </si>
+  <si>
+    <t>BAT Pushbuttons .................................................................. OFF</t>
+  </si>
+  <si>
+    <t>*** Nếu vẫn không dập cháy được, NVKT báo cho cứu hỏa chi nhánh Vaeco phía nam (SĐT: 028.38.488.438) và đội cứu hỏa sân bay TSN (SĐT: 028.38.485.383-3208) để hỗ trợ</t>
+  </si>
+  <si>
+    <t>INTERNAL/EXHAUST ENGINE FIREStrictly performed IAW approved maintenance data/procedure and strictly follow engine safety precautions</t>
+  </si>
+  <si>
+    <t>Thông báo cho cockpit man bằng cáp/ bộ đàm/ hand signal động cơ nào cháy/khói</t>
+  </si>
+  <si>
+    <t>Cockpit Man</t>
+  </si>
+  <si>
+    <t>CO-ERU CALL MECH, SGNBASE…………..CONFIRM WHICH ENG FIRE.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thrust Levers (both) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>......................................................... IDLE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ENG MASTER Switch (affected engine)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>........................ OFF</t>
+    </r>
+  </si>
+  <si>
+    <t>Checked if Internal/Exhaust Engine Fire is fully extinguished and report to Cockpit Man.</t>
+  </si>
+  <si>
+    <t>Checked EGT on affected engine reduce.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ENGINE MANUAL START (affected engine) P/B </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>........OFF</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ENG MODE Selector </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>................................................. NORM</t>
+    </r>
+  </si>
+  <si>
+    <t>If the engine motoring does not extinguish the fire or if the engine motoring is not possible do the following:</t>
+  </si>
+  <si>
+    <r>
+      <t>ENG FIRE P/B (affected engine)…………………</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>RELEASE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>LP VALVE (affected engine) on FUEL PAGE……</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>CLOSED</t>
+    </r>
+  </si>
+  <si>
+    <t>REQUEST HEADSET MAN AND FIRE GUARD TO EXTINGUISH THE FIRE WITH FIRE BOTTLE (CO2).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Headset Man </t>
+  </si>
+  <si>
+    <t>Yêu cầu nhân viên trực cứu hỏa (Fire Guard) tiến hành xịt dập cháy động cơ bằng bình CO2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fire Guard </t>
+  </si>
+  <si>
+    <t>NV trực cứu hỏa tiếp cận xịt bình cứu hỏa CO2 từ phía sau vào EXHAUST của động cơ.</t>
+  </si>
+  <si>
+    <t>*** Nếu vẫn không dập cháy được, NVKT báo cho cứu hỏa chi nhánh Vaeco phía nam (SĐT: 028.38.488.438) và đội cứu hỏa sân bay TSN (SĐT: 028.38.485.383-3208) để hỗ trợ.</t>
+  </si>
+  <si>
+    <r>
+      <t>AIRCRAFT IS MOVING WHEN ENGINE IS RUNNING</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Strictly performed IAW approved maintenance data/procedure and strictly follow engine safety precautions</t>
+    </r>
+  </si>
+  <si>
+    <t>Thông báo cho NVKT trên cockpit bằng cáp/bộ đàm/hand signal.</t>
+  </si>
+  <si>
+    <t>Di chuyển tránh khỏi đường di chuyển của máy bay theo hướng lệc về trái/phải – hướng về trước (TRÁNH CHẠY VÀO ĐỘNG CƠ).</t>
+  </si>
+  <si>
+    <t>Thông báo cho nhân viên cảnh giới Ground Observer chuẩn bị chèn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ground Observer </t>
+  </si>
+  <si>
+    <t>Chuẩn bị sẵn sàng chèn máy bay khi máy bay đã dừng hoặc di chuyển rất chậm; và động cơ đã tắt.</t>
+  </si>
+  <si>
+    <r>
+      <t>THRUST LEVERS..................................................</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>IDLE/STOWED.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Steering Handwheel……………………………</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>TURN (As require).</t>
+    </r>
+  </si>
+  <si>
+    <t>Đến khi tàu bay dừng hẳn hoặc di chuyển rất chậm.</t>
+  </si>
+  <si>
+    <t>Nếu hệ thống phanh hỏng, không phanh máy bay được thì:</t>
+  </si>
+  <si>
+    <t>BRAKE Pedals…………………………….….………..APPLY.</t>
+  </si>
+  <si>
+    <t>BRAKE Pedals…………………………….….……RE-APPLY.</t>
+  </si>
+  <si>
+    <t>REV Thrust Levers………………….……………… REV IF REQ.</t>
+  </si>
+  <si>
+    <t>Master Switch both ENG…………..……………..…..........OFF.</t>
+  </si>
+  <si>
+    <t>Confirm with Cockpit Man: ENGINE OFF.</t>
+  </si>
+  <si>
+    <t>Yêu cầu nhân viên mặt đất tiếp cận càng chính, dùng chèn để chèn máy bay.</t>
+  </si>
+  <si>
+    <t>Ground Observer</t>
+  </si>
+  <si>
+    <t>Tiếp cận càng chính, dùng chèn để chèn máy bay.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cockpit Lighting ....................................................... As required
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Dome light should be selected on as it is available in EMER ELEC configuration.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ADIRS Mode Rotary Selectors ...............................................NAV
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>IRS IN ALIGN&gt; 7MN appears on ECAM MEMO page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fuel On Board (ECAM E/WD)............................................. NOTE
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Calculate Fuel Qty to make sure after engine shutdown there should be at least 3000 kgs of fuel on board for stability reasons.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RMP 2 ................................................................................. Check ON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>. 
+SEL and NAV lights extinguished.
+. Set frequencies as required.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ACP 2 .............................................................................................. INT
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>· Check transmission and reception with ground crew.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FLAPS Lever Position ......................................................... CHECK
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>If lever does not agree with flaps/slats indication on ECAM E/WD, set flaps lever to corresponding position.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ECAM Control Panel .....................................................Select HYD
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Check hydraulic quantities in normal range, no AIR LOW PRESS warnings.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ECAM Control Panel ................................................... Select FUEL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Check fuel distribution.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ECAM Control Panel ...................................................... Select STS
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Check if inoperable systems are compatible for engine run-up.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ECAM Control Panel ......................................................Select CLR
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Select CLR as many times as necessary until ECAM DOOR/OXY page appears.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PARKING BRK ............................................................................. ON
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Check parking brake pressure indication normal.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MCDU 1 (2)..................................................................................... ON
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Check data base validity.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MCDU ............................................................................... Select INIT
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Insert airport ICAO reference using keyboard. (VVTS/VVTS for SGN station)MCDU/INIT, select Next Page.Select ALIGN IRS prompt to complete IRS alignment.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ENG 1 (2) FIRE TEST ............................. PERFORM
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>- Check:
+. ENG 1 (2) FIRE pushbutton light illuminates.
+· SQUIB and DISCH lights illuminate.
+· MASTER WARNING illuminated.
+· ENG 1 (2) FIRE warning on ECAM E/WD.
+. CRC sounds.
+. ECAM ENG page appears.
+. FIRE 1 (2) light illuminates.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FADEC Ground Power (both)........................... ON
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>· On E/WD, check all indications normal.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ECAM Control Panel ..............................Select ENG
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>· Check all engine parameters for logical indication and sufficient oil quantity.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ECAM Control Panel ..............................Select ENG
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>· ECAM DOOR/OXY page appears, check all doors closed.</t>
+    </r>
+  </si>
+  <si>
+    <t>FADEC Ground Power (both) .........................OFF
+ATC Clearance ............................................. OBTAIN</t>
+  </si>
+  <si>
+    <t>APU BLEED or HOT AIR BLEED (If APU is INOP)………..ON
+Check Bleed Air Pressure is sufficient for Dry Crank.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thrust Levers (both).......................................................... IDLE
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
       <t>. During engine spool down, advise ground crew of the situation, and notify ATC.</t>
     </r>
   </si>
   <si>
-    <t>PARKING BRK ...................................................................... ON</t>
-  </si>
-  <si>
-    <r>
-      <t>ENG MASTER Switch (affected engine)........................... OFF</t>
+    <r>
+      <t xml:space="preserve">ENG MASTER Switch (affected engine)........................... OFF
+</t>
     </r>
     <r>
       <rPr>
@@ -915,7 +1144,8 @@
   </si>
   <si>
     <r>
-      <t>ENG FIRE Pushbutton (affected engine) ............... RELEASE</t>
+      <t xml:space="preserve">ENG FIRE Pushbutton (affected engine) ............... RELEASE
+</t>
     </r>
     <r>
       <rPr>
@@ -924,72 +1154,28 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>. AGENT lights illuminate.. Aural warning cancelled.Note: Visual warnings remain illuminated as long as fire is detected.</t>
-    </r>
-  </si>
-  <si>
-    <t>AGENT 1 &amp; 2 Pushbutton (affected engine)..................PRESS</t>
-  </si>
-  <si>
-    <t>ENG MASTER Switch (other engine) ............................... OFF</t>
-  </si>
-  <si>
-    <t>If Fire Warnings persist:CO-ERU CALL MECH……………….…GROUND FIRE BOTTLE (CO2) READY TO EXTINGUISH EXTERNAL FIRE SOURCE (DO NOT LET AGENTS GO INTO ENG INLET/EXHAUST).REQUEST HEADSET MAN AND FIRE GUARD TO EXTINGUISH THE FIRE.</t>
-  </si>
-  <si>
-    <t>Quan sát động cơ, nếu hiện tượng cháy vẫn tiếp tục và lan ra phía ngoài cowl động cơ, Headset man cho triển khai phun dập cháy từ bên ngoài động cơ.</t>
-  </si>
-  <si>
-    <t>Yêu cầu nhân viên trực cứu hỏa (Fire Guard) tiến hành dập cháy động cơ.</t>
-  </si>
-  <si>
-    <t>Fire Guard</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">NV trực cứu hỏa tiếp cận xịt bình cứu hỏa CO2 vào khu vực cháy trên động cơ. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t>. AGENT lights illuminate.
+. Aural warning cancelled
+.Note: Visual warnings remain illuminated as long as fire is detected.</t>
+    </r>
+  </si>
+  <si>
+    <t>If Fire Warnings persist:CO-ERU CALL MECH……………….…GROUND FIRE BOTTLE (CO2) READY TO EXTINGUISH EXTERNAL FIRE SOURCE (DO NOT LET AGENTS GO INTO ENG INLET/EXHAUST)
+.REQUEST HEADSET MAN AND FIRE GUARD TO EXTINGUISH THE FIRE.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) IF APU BLEED AVAILABLE:
+</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Lưu ý không xịt vào Engine Inlet/Exhaust.</t>
-    </r>
-  </si>
-  <si>
-    <t>APU FIRE Pushbutton ............................................. RELEASE</t>
-  </si>
-  <si>
-    <t>ADIRS Mode Rotary Selectors ........................................... OFF</t>
-  </si>
-  <si>
-    <t>EXT PWR Pushbutton ........................................................ OFF</t>
-  </si>
-  <si>
-    <t>BAT Pushbuttons .................................................................. OFF</t>
-  </si>
-  <si>
-    <t>*** Nếu vẫn không dập cháy được, NVKT báo cho cứu hỏa chi nhánh Vaeco phía nam (SĐT: 028.38.488.438) và đội cứu hỏa sân bay TSN (SĐT: 028.38.485.383-3208) để hỗ trợ</t>
-  </si>
-  <si>
-    <t>INTERNAL/EXHAUST ENGINE FIREStrictly performed IAW approved maintenance data/procedure and strictly follow engine safety precautions</t>
-  </si>
-  <si>
-    <t>Thông báo cho cockpit man bằng cáp/ bộ đàm/ hand signal động cơ nào cháy/khói</t>
-  </si>
-  <si>
-    <t>Cockpit Man</t>
-  </si>
-  <si>
-    <t>CO-ERU CALL MECH, SGNBASE…………..CONFIRM WHICH ENG FIRE.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Thrust Levers (both) </t>
+      <t xml:space="preserve">APU BLEED Pushbutton </t>
     </r>
     <r>
       <rPr>
@@ -999,59 +1185,86 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>......................................................... IDLE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ENG MASTER Switch (affected engine)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t>.................................................. ON</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2) IF APU BLEED NOT AVAILABLE:
+</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>........................ OFF</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1) IF APU BLEED AVAILABLE:</t>
-    </r>
-    <r>
-      <rPr>
+      <t>X BLEED Valve Selector</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">APU BLEED Pushbutton </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t xml:space="preserve">............................................. OPEN
+</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>.................................................. ON</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2) IF APU BLEED NOT AVAILABLE:</t>
-    </r>
-    <r>
-      <rPr>
+      <t xml:space="preserve">ENG BLEED (running engine) Pushbutton </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
+      <t>...................... ON</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3) IF APU BLEED AND ENGINE BLEED NOT AVAILABLE:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">External Pneumatic Power </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">........................................ Connect
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
       <t>X BLEED Valve Selector</t>
     </r>
     <r>
@@ -1062,7 +1275,8 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>............................................. OPEN</t>
+      <t xml:space="preserve">.................................... As required
+</t>
     </r>
     <r>
       <rPr>
@@ -1071,7 +1285,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">ENG BLEED (running engine) Pushbutton </t>
+      <t xml:space="preserve">ENG MODE Selector </t>
     </r>
     <r>
       <rPr>
@@ -1081,12 +1295,8 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>...................... ON</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>3) IF APU BLEED AND ENGINE BLEED NOT AVAILABLE:</t>
+      <t xml:space="preserve">................................................ CRANK
+</t>
     </r>
     <r>
       <rPr>
@@ -1095,7 +1305,8 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">External Pneumatic Power </t>
+      <t xml:space="preserve">. Check AIR PRESS above 30 psi.
+Engine Manual Start (affected engine) Pushbutton </t>
     </r>
     <r>
       <rPr>
@@ -1105,7 +1316,8 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>........................................ Connect</t>
+      <t xml:space="preserve">........... ON
+</t>
     </r>
     <r>
       <rPr>
@@ -1114,7 +1326,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>X BLEED Valve Selector</t>
+      <t xml:space="preserve">Note: Dry Motor engine until you remove all indications related to fire. </t>
     </r>
     <r>
       <rPr>
@@ -1124,242 +1336,8 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>.................................... As required</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">ENG MODE Selector </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>................................................ CRANK</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">. Check AIR PRESS above 30 psi.Engine Manual Start (affected engine) Pushbutton </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>........... ON</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Note: Dry Motor engine until you remove all indications related to fire. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>Ignore the starter time limits.</t>
     </r>
-  </si>
-  <si>
-    <t>Checked if Internal/Exhaust Engine Fire is fully extinguished and report to Cockpit Man.</t>
-  </si>
-  <si>
-    <t>Checked EGT on affected engine reduce.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ENGINE MANUAL START (affected engine) P/B </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>........OFF</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ENG MODE Selector </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>................................................. NORM</t>
-    </r>
-  </si>
-  <si>
-    <t>If the engine motoring does not extinguish the fire or if the engine motoring is not possible do the following:</t>
-  </si>
-  <si>
-    <r>
-      <t>ENG FIRE P/B (affected engine)…………………</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>RELEASE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>LP VALVE (affected engine) on FUEL PAGE……</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>CLOSED</t>
-    </r>
-  </si>
-  <si>
-    <t>REQUEST HEADSET MAN AND FIRE GUARD TO EXTINGUISH THE FIRE WITH FIRE BOTTLE (CO2).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Headset Man </t>
-  </si>
-  <si>
-    <t>Yêu cầu nhân viên trực cứu hỏa (Fire Guard) tiến hành xịt dập cháy động cơ bằng bình CO2.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fire Guard </t>
-  </si>
-  <si>
-    <t>NV trực cứu hỏa tiếp cận xịt bình cứu hỏa CO2 từ phía sau vào EXHAUST của động cơ.</t>
-  </si>
-  <si>
-    <t>*** Nếu vẫn không dập cháy được, NVKT báo cho cứu hỏa chi nhánh Vaeco phía nam (SĐT: 028.38.488.438) và đội cứu hỏa sân bay TSN (SĐT: 028.38.485.383-3208) để hỗ trợ.</t>
-  </si>
-  <si>
-    <r>
-      <t>AIRCRAFT IS MOVING WHEN ENGINE IS RUNNING</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Strictly performed IAW approved maintenance data/procedure and strictly follow engine safety precautions</t>
-    </r>
-  </si>
-  <si>
-    <t>Thông báo cho NVKT trên cockpit bằng cáp/bộ đàm/hand signal.</t>
-  </si>
-  <si>
-    <t>Di chuyển tránh khỏi đường di chuyển của máy bay theo hướng lệc về trái/phải – hướng về trước (TRÁNH CHẠY VÀO ĐỘNG CƠ).</t>
-  </si>
-  <si>
-    <t>Thông báo cho nhân viên cảnh giới Ground Observer chuẩn bị chèn.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ground Observer </t>
-  </si>
-  <si>
-    <t>Chuẩn bị sẵn sàng chèn máy bay khi máy bay đã dừng hoặc di chuyển rất chậm; và động cơ đã tắt.</t>
-  </si>
-  <si>
-    <r>
-      <t>THRUST LEVERS..................................................</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>IDLE/STOWED.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Steering Handwheel……………………………</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>TURN (As require).</t>
-    </r>
-  </si>
-  <si>
-    <t>Đến khi tàu bay dừng hẳn hoặc di chuyển rất chậm.</t>
-  </si>
-  <si>
-    <t>Nếu hệ thống phanh hỏng, không phanh máy bay được thì:</t>
-  </si>
-  <si>
-    <t>BRAKE Pedals…………………………….….………..APPLY.</t>
-  </si>
-  <si>
-    <t>BRAKE Pedals…………………………….….……RE-APPLY.</t>
-  </si>
-  <si>
-    <t>REV Thrust Levers………………….……………… REV IF REQ.</t>
-  </si>
-  <si>
-    <t>Master Switch both ENG…………..……………..…..........OFF.</t>
-  </si>
-  <si>
-    <t>Confirm with Cockpit Man: ENGINE OFF.</t>
-  </si>
-  <si>
-    <t>Yêu cầu nhân viên mặt đất tiếp cận càng chính, dùng chèn để chèn máy bay.</t>
-  </si>
-  <si>
-    <t>Ground Observer</t>
-  </si>
-  <si>
-    <t>Tiếp cận càng chính, dùng chèn để chèn máy bay.</t>
   </si>
 </sst>
 </file>
@@ -1838,15 +1816,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234709FA-C916-4334-B86D-527E577F47AF}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="51.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="56.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="76.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.3">
@@ -1911,68 +1890,68 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5"/>
     </row>
@@ -1990,166 +1969,117 @@
       </c>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="2" t="s">
-        <v>24</v>
+        <v>122</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>123</v>
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
-        <v>27</v>
+        <v>124</v>
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>31</v>
+        <v>126</v>
       </c>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>32</v>
+        <v>127</v>
       </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>34</v>
+        <v>129</v>
       </c>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>35</v>
+        <v>130</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
-        <v>37</v>
+        <v>131</v>
       </c>
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="2" t="s">
-        <v>38</v>
+        <v>132</v>
       </c>
       <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" s="5"/>
-    </row>
-    <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="5"/>
-    </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="5"/>
-    </row>
-    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-      <c r="B41" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" s="5"/>
-    </row>
-    <row r="42" spans="1:3" ht="75" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-      <c r="B42" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2163,8 +2093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5BF4F8-3348-478C-80C8-66F4B554B0FF}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2176,7 +2106,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -2194,223 +2124,223 @@
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="135" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>133</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>134</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>135</v>
       </c>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>136</v>
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>137</v>
       </c>
       <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="2" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="2" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="4" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="4" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="4" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="4" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="4" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="4" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="4" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="4" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="4" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="4" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="4" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="4" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="4" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="4" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="34" spans="1:3" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -2428,35 +2358,35 @@
     </row>
     <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B40" s="3" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -2474,50 +2404,50 @@
     </row>
     <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B45" s="3" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B46" s="7" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B47" s="3" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="B48" s="7" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B49" s="3" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="30" x14ac:dyDescent="0.3">
       <c r="B50" s="3" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B51" s="3" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B52" s="3" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2534,15 +2464,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6867C1-899A-412B-9201-869842C9E604}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="72.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2560,97 +2494,97 @@
     </row>
     <row r="3" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>98</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
-        <v>99</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="93.6" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
-        <v>102</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2665,20 +2599,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61136C37-7AA2-45B5-935B-7C4537A69A51}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.33203125" customWidth="1"/>
-    <col min="2" max="2" width="59" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="67.33203125" customWidth="1"/>
     <col min="3" max="3" width="69" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2696,113 +2630,113 @@
     </row>
     <row r="3" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2830,7 +2764,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -2848,92 +2782,92 @@
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding some key elements
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Coding\Project\python\Self-Project\ordered\Checklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655D49FD-A239-4441-9B74-C2AC7992685C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F82738-2E2E-423A-954D-97BD65CA7048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7344" yWindow="0" windowWidth="15312" windowHeight="12240" firstSheet="2" activeTab="4" xr2:uid="{B679EF15-A35F-43FE-B7D2-F2BE67EA73A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{B679EF15-A35F-43FE-B7D2-F2BE67EA73A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Trước khi nổ máy" sheetId="1" r:id="rId1"/>
@@ -150,20 +150,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Scan Sequence ............................................................. PERFORM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Note: During the scan sequence, it is a general rule to extinguish all white lights on the overhead panel except PACKS &amp; FUEL PUMPS and to set all the rotary selectors to the NORM/AUTO (12 o'clock) position.</t>
-    </r>
-  </si>
-  <si>
     <t>ANN LT Test ................................................................ PERFORM</t>
   </si>
   <si>
@@ -1020,21 +1006,6 @@
         <family val="1"/>
       </rPr>
       <t>Check data base validity.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">MCDU ............................................................................... Select INIT
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Insert airport ICAO reference using keyboard. (VVTS/VVTS for SGN station)MCDU/INIT, select Next Page.Select ALIGN IRS prompt to complete IRS alignment.</t>
     </r>
   </si>
   <si>
@@ -1337,6 +1308,37 @@
         <family val="1"/>
       </rPr>
       <t>Ignore the starter time limits.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Scan Sequence ............................................................. PERFORM 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Note: During the scan sequence, it is a general rule to extinguish all white lights on the overhead panel except PACKS &amp; FUEL PUMPS and to set all the rotary selectors to the NORM/AUTO (12 o'clock) position.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MCDU ............................................................................... Select INIT
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Insert airport ICAO reference using keyboard. (VVTS/VVTS for SGN station)MCDU/INIT, select Next Page
+.Select ALIGN IRS prompt to complete IRS alignment.</t>
     </r>
   </si>
 </sst>
@@ -1441,7 +1443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1477,10 +1479,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1818,25 +1830,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234709FA-C916-4334-B86D-527E577F47AF}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="51.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="76.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1847,7 +1859,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1856,228 +1868,228 @@
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
+      <c r="B10" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A11" s="15"/>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A13" s="15"/>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+      <c r="B17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A18" s="15"/>
+      <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2" t="s">
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A21" s="15"/>
+      <c r="B21" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A22" s="15"/>
+      <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2" t="s">
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A23" s="15"/>
+      <c r="B23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2" t="s">
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A24" s="15"/>
+      <c r="B24" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A25" s="15"/>
+      <c r="B25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2" t="s">
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A26" s="15"/>
+      <c r="B26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A27" s="15"/>
+      <c r="B27" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2" t="s">
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
+      <c r="B28" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A29" s="15"/>
+      <c r="B29" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A30" s="15"/>
+      <c r="B30" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A31" s="15"/>
+      <c r="B31" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A32" s="15"/>
+      <c r="B32" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A33" s="15"/>
+      <c r="B33" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="5"/>
-    </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2" t="s">
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A34" s="15"/>
+      <c r="B34" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3" ht="60" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="2" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="C35" s="5"/>
     </row>
@@ -2093,26 +2105,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5BF4F8-3348-478C-80C8-66F4B554B0FF}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A44" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.6640625" customWidth="1"/>
     <col min="3" max="3" width="47.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="A1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2123,230 +2135,230 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>19</v>
+      <c r="A3" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" ht="135" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="34" spans="1:3" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
+      <c r="A34" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
     </row>
     <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -2357,42 +2369,42 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>38</v>
+      <c r="A36" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B40" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
     </row>
     <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -2403,51 +2415,51 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>38</v>
+      <c r="A44" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B45" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B46" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B47" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="B48" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B49" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="30" x14ac:dyDescent="0.3">
       <c r="B50" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B51" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B52" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2465,7 +2477,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A8" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2475,11 +2487,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="A1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2494,97 +2506,97 @@
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="93.6" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>76</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2600,25 +2612,25 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B10" sqref="B1:B1048576"/>
+      <selection activeCell="A10" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.33203125" customWidth="1"/>
     <col min="3" max="3" width="69" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="A1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -2629,114 +2641,114 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>36</v>
+      <c r="A3" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="B4" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>36</v>
+      <c r="A10" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="B18" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B18" s="10" t="s">
+    </row>
+    <row r="19" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="B19" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="10" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="48.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="48.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2752,25 +2764,25 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.77734375" customWidth="1"/>
     <col min="3" max="3" width="65.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="A1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2781,93 +2793,93 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>36</v>
+      <c r="A3" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>85</v>
+      <c r="A7" s="15" t="s">
+        <v>84</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>